<commit_message>
finished ocean_doc sheet structure
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48602ECA-85DF-44BE-AC16-FC6E98BB717B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C73561-EC19-434C-837C-6B6F4E1E8011}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -747,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -774,22 +774,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -828,16 +822,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -891,6 +882,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1370,7 +1371,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomRight" activeCell="AW3" sqref="AW3:BS3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.58203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1660,231 +1661,231 @@
     </row>
     <row r="2" spans="1:140" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9"/>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="34" t="s">
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="37" t="s">
+      <c r="Q2" s="33"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="28" t="s">
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="31" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="34" t="s">
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="AN2" s="35"/>
-      <c r="AO2" s="36"/>
-      <c r="AP2" s="37" t="s">
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="AQ2" s="38"/>
-      <c r="AR2" s="38"/>
-      <c r="AS2" s="38"/>
-      <c r="AT2" s="38"/>
-      <c r="AU2" s="38"/>
-      <c r="AV2" s="39"/>
-      <c r="AW2" s="28" t="s">
+      <c r="AQ2" s="36"/>
+      <c r="AR2" s="36"/>
+      <c r="AS2" s="36"/>
+      <c r="AT2" s="36"/>
+      <c r="AU2" s="36"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AX2" s="29"/>
-      <c r="AY2" s="29"/>
-      <c r="AZ2" s="29"/>
-      <c r="BA2" s="29"/>
-      <c r="BB2" s="29"/>
-      <c r="BC2" s="30"/>
-      <c r="BD2" s="31" t="s">
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="28"/>
+      <c r="BD2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="32"/>
-      <c r="BG2" s="32"/>
-      <c r="BH2" s="32"/>
-      <c r="BI2" s="33"/>
-      <c r="BJ2" s="34" t="s">
+      <c r="BE2" s="30"/>
+      <c r="BF2" s="30"/>
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="31"/>
+      <c r="BJ2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="BK2" s="35"/>
-      <c r="BL2" s="36"/>
-      <c r="BM2" s="37" t="s">
+      <c r="BK2" s="33"/>
+      <c r="BL2" s="34"/>
+      <c r="BM2" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="BN2" s="38"/>
-      <c r="BO2" s="38"/>
-      <c r="BP2" s="38"/>
-      <c r="BQ2" s="38"/>
-      <c r="BR2" s="38"/>
-      <c r="BS2" s="39"/>
-      <c r="BT2" s="28" t="s">
+      <c r="BN2" s="36"/>
+      <c r="BO2" s="36"/>
+      <c r="BP2" s="36"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="36"/>
+      <c r="BS2" s="37"/>
+      <c r="BT2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="BU2" s="29"/>
-      <c r="BV2" s="29"/>
-      <c r="BW2" s="29"/>
-      <c r="BX2" s="29"/>
-      <c r="BY2" s="29"/>
-      <c r="BZ2" s="30"/>
-      <c r="CA2" s="31" t="s">
+      <c r="BU2" s="27"/>
+      <c r="BV2" s="27"/>
+      <c r="BW2" s="27"/>
+      <c r="BX2" s="27"/>
+      <c r="BY2" s="27"/>
+      <c r="BZ2" s="28"/>
+      <c r="CA2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="CB2" s="32"/>
-      <c r="CC2" s="32"/>
-      <c r="CD2" s="32"/>
-      <c r="CE2" s="32"/>
-      <c r="CF2" s="33"/>
-      <c r="CG2" s="34" t="s">
+      <c r="CB2" s="30"/>
+      <c r="CC2" s="30"/>
+      <c r="CD2" s="30"/>
+      <c r="CE2" s="30"/>
+      <c r="CF2" s="31"/>
+      <c r="CG2" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="CH2" s="35"/>
-      <c r="CI2" s="36"/>
-      <c r="CJ2" s="37" t="s">
+      <c r="CH2" s="33"/>
+      <c r="CI2" s="34"/>
+      <c r="CJ2" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="CK2" s="38"/>
-      <c r="CL2" s="38"/>
-      <c r="CM2" s="38"/>
-      <c r="CN2" s="38"/>
-      <c r="CO2" s="38"/>
-      <c r="CP2" s="39"/>
+      <c r="CK2" s="36"/>
+      <c r="CL2" s="36"/>
+      <c r="CM2" s="36"/>
+      <c r="CN2" s="36"/>
+      <c r="CO2" s="36"/>
+      <c r="CP2" s="37"/>
     </row>
     <row r="3" spans="1:140" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="40" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="AA3" s="41"/>
-      <c r="AB3" s="41"/>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="41"/>
-      <c r="AE3" s="41"/>
-      <c r="AF3" s="41"/>
-      <c r="AG3" s="41"/>
-      <c r="AH3" s="41"/>
-      <c r="AI3" s="41"/>
-      <c r="AJ3" s="41"/>
-      <c r="AK3" s="41"/>
-      <c r="AL3" s="41"/>
-      <c r="AM3" s="41"/>
-      <c r="AN3" s="41"/>
-      <c r="AO3" s="41"/>
-      <c r="AP3" s="41"/>
-      <c r="AQ3" s="41"/>
-      <c r="AR3" s="41"/>
-      <c r="AS3" s="41"/>
-      <c r="AT3" s="41"/>
-      <c r="AU3" s="41"/>
-      <c r="AV3" s="42"/>
-      <c r="AW3" s="40" t="s">
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AX3" s="41"/>
-      <c r="AY3" s="41"/>
-      <c r="AZ3" s="41"/>
-      <c r="BA3" s="41"/>
-      <c r="BB3" s="41"/>
-      <c r="BC3" s="41"/>
-      <c r="BD3" s="41"/>
-      <c r="BE3" s="41"/>
-      <c r="BF3" s="41"/>
-      <c r="BG3" s="41"/>
-      <c r="BH3" s="41"/>
-      <c r="BI3" s="41"/>
-      <c r="BJ3" s="41"/>
-      <c r="BK3" s="41"/>
-      <c r="BL3" s="41"/>
-      <c r="BM3" s="41"/>
-      <c r="BN3" s="41"/>
-      <c r="BO3" s="41"/>
-      <c r="BP3" s="41"/>
-      <c r="BQ3" s="41"/>
-      <c r="BR3" s="41"/>
-      <c r="BS3" s="42"/>
-      <c r="BT3" s="40" t="s">
+      <c r="AX3" s="23"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="23"/>
+      <c r="BE3" s="23"/>
+      <c r="BF3" s="23"/>
+      <c r="BG3" s="23"/>
+      <c r="BH3" s="23"/>
+      <c r="BI3" s="23"/>
+      <c r="BJ3" s="23"/>
+      <c r="BK3" s="23"/>
+      <c r="BL3" s="23"/>
+      <c r="BM3" s="23"/>
+      <c r="BN3" s="23"/>
+      <c r="BO3" s="23"/>
+      <c r="BP3" s="23"/>
+      <c r="BQ3" s="23"/>
+      <c r="BR3" s="23"/>
+      <c r="BS3" s="24"/>
+      <c r="BT3" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="BU3" s="41"/>
-      <c r="BV3" s="41"/>
-      <c r="BW3" s="41"/>
-      <c r="BX3" s="41"/>
-      <c r="BY3" s="41"/>
-      <c r="BZ3" s="41"/>
-      <c r="CA3" s="41"/>
-      <c r="CB3" s="41"/>
-      <c r="CC3" s="41"/>
-      <c r="CD3" s="41"/>
-      <c r="CE3" s="41"/>
-      <c r="CF3" s="41"/>
-      <c r="CG3" s="41"/>
-      <c r="CH3" s="41"/>
-      <c r="CI3" s="41"/>
-      <c r="CJ3" s="41"/>
-      <c r="CK3" s="41"/>
-      <c r="CL3" s="41"/>
-      <c r="CM3" s="41"/>
-      <c r="CN3" s="41"/>
-      <c r="CO3" s="41"/>
-      <c r="CP3" s="43"/>
+      <c r="BU3" s="23"/>
+      <c r="BV3" s="23"/>
+      <c r="BW3" s="23"/>
+      <c r="BX3" s="23"/>
+      <c r="BY3" s="23"/>
+      <c r="BZ3" s="23"/>
+      <c r="CA3" s="23"/>
+      <c r="CB3" s="23"/>
+      <c r="CC3" s="23"/>
+      <c r="CD3" s="23"/>
+      <c r="CE3" s="23"/>
+      <c r="CF3" s="23"/>
+      <c r="CG3" s="23"/>
+      <c r="CH3" s="23"/>
+      <c r="CI3" s="23"/>
+      <c r="CJ3" s="23"/>
+      <c r="CK3" s="23"/>
+      <c r="CL3" s="23"/>
+      <c r="CM3" s="23"/>
+      <c r="CN3" s="23"/>
+      <c r="CO3" s="23"/>
+      <c r="CP3" s="25"/>
     </row>
     <row r="4" spans="1:140" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
@@ -2200,7 +2201,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="R6" s="61"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -4808,6 +4809,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C3:Y3"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="Z2:AF2"/>
+    <mergeCell ref="AG2:AL2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="AP2:AV2"/>
+    <mergeCell ref="Z3:AV3"/>
     <mergeCell ref="AW3:BS3"/>
     <mergeCell ref="BT3:CP3"/>
     <mergeCell ref="AW2:BC2"/>
@@ -4818,16 +4829,6 @@
     <mergeCell ref="CA2:CF2"/>
     <mergeCell ref="CG2:CI2"/>
     <mergeCell ref="CJ2:CP2"/>
-    <mergeCell ref="Z2:AF2"/>
-    <mergeCell ref="AG2:AL2"/>
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="AP2:AV2"/>
-    <mergeCell ref="Z3:AV3"/>
-    <mergeCell ref="C3:Y3"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:Y2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4855,18 +4856,18 @@
   <sheetData>
     <row r="1" spans="3:151" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:151" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="60"/>
     </row>
     <row r="4" spans="3:151" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
@@ -5144,221 +5145,221 @@
     </row>
     <row r="11" spans="3:151" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M11" s="9"/>
-      <c r="N11" s="28" t="s">
+      <c r="N11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="31" t="s">
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
-      <c r="X11" s="32"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="34" t="s">
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="31"/>
+      <c r="AA11" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="AB11" s="35"/>
-      <c r="AC11" s="36"/>
-      <c r="AD11" s="37" t="s">
+      <c r="AB11" s="33"/>
+      <c r="AC11" s="34"/>
+      <c r="AD11" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="AE11" s="38"/>
-      <c r="AF11" s="38"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
-      <c r="AI11" s="38"/>
-      <c r="AJ11" s="39"/>
-      <c r="AK11" s="28" t="s">
+      <c r="AE11" s="36"/>
+      <c r="AF11" s="36"/>
+      <c r="AG11" s="36"/>
+      <c r="AH11" s="36"/>
+      <c r="AI11" s="36"/>
+      <c r="AJ11" s="37"/>
+      <c r="AK11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AL11" s="29"/>
-      <c r="AM11" s="29"/>
-      <c r="AN11" s="29"/>
-      <c r="AO11" s="29"/>
-      <c r="AP11" s="29"/>
-      <c r="AQ11" s="30"/>
-      <c r="AR11" s="31" t="s">
+      <c r="AL11" s="27"/>
+      <c r="AM11" s="27"/>
+      <c r="AN11" s="27"/>
+      <c r="AO11" s="27"/>
+      <c r="AP11" s="27"/>
+      <c r="AQ11" s="28"/>
+      <c r="AR11" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="AS11" s="32"/>
-      <c r="AT11" s="32"/>
-      <c r="AU11" s="32"/>
-      <c r="AV11" s="32"/>
-      <c r="AW11" s="33"/>
-      <c r="AX11" s="34" t="s">
+      <c r="AS11" s="30"/>
+      <c r="AT11" s="30"/>
+      <c r="AU11" s="30"/>
+      <c r="AV11" s="30"/>
+      <c r="AW11" s="31"/>
+      <c r="AX11" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="AY11" s="35"/>
-      <c r="AZ11" s="36"/>
-      <c r="BA11" s="37" t="s">
+      <c r="AY11" s="33"/>
+      <c r="AZ11" s="34"/>
+      <c r="BA11" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="BB11" s="38"/>
-      <c r="BC11" s="38"/>
-      <c r="BD11" s="38"/>
-      <c r="BE11" s="38"/>
-      <c r="BF11" s="38"/>
-      <c r="BG11" s="38"/>
-      <c r="BH11" s="48" t="s">
+      <c r="BB11" s="36"/>
+      <c r="BC11" s="36"/>
+      <c r="BD11" s="36"/>
+      <c r="BE11" s="36"/>
+      <c r="BF11" s="36"/>
+      <c r="BG11" s="36"/>
+      <c r="BH11" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="BI11" s="49"/>
-      <c r="BJ11" s="49"/>
-      <c r="BK11" s="49"/>
-      <c r="BL11" s="49"/>
-      <c r="BM11" s="49"/>
-      <c r="BN11" s="50"/>
-      <c r="BO11" s="51" t="s">
+      <c r="BI11" s="46"/>
+      <c r="BJ11" s="46"/>
+      <c r="BK11" s="46"/>
+      <c r="BL11" s="46"/>
+      <c r="BM11" s="46"/>
+      <c r="BN11" s="47"/>
+      <c r="BO11" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="BP11" s="52"/>
-      <c r="BQ11" s="52"/>
-      <c r="BR11" s="52"/>
-      <c r="BS11" s="52"/>
-      <c r="BT11" s="53"/>
-      <c r="BU11" s="54" t="s">
+      <c r="BP11" s="49"/>
+      <c r="BQ11" s="49"/>
+      <c r="BR11" s="49"/>
+      <c r="BS11" s="49"/>
+      <c r="BT11" s="50"/>
+      <c r="BU11" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="BV11" s="55"/>
-      <c r="BW11" s="56"/>
-      <c r="BX11" s="57" t="s">
+      <c r="BV11" s="52"/>
+      <c r="BW11" s="53"/>
+      <c r="BX11" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="BY11" s="58"/>
-      <c r="BZ11" s="58"/>
-      <c r="CA11" s="58"/>
-      <c r="CB11" s="58"/>
-      <c r="CC11" s="58"/>
-      <c r="CD11" s="59"/>
-      <c r="CE11" s="47"/>
-      <c r="CF11" s="47"/>
-      <c r="CG11" s="47"/>
-      <c r="CH11" s="47"/>
-      <c r="CI11" s="47"/>
-      <c r="CJ11" s="47"/>
-      <c r="CK11" s="47"/>
-      <c r="CL11" s="47"/>
-      <c r="CM11" s="47"/>
-      <c r="CN11" s="47"/>
-      <c r="CO11" s="47"/>
-      <c r="CP11" s="47"/>
-      <c r="CQ11" s="47"/>
-      <c r="CR11" s="60"/>
-      <c r="CS11" s="60"/>
-      <c r="CT11" s="60"/>
-      <c r="CU11" s="47"/>
-      <c r="CV11" s="47"/>
-      <c r="CW11" s="47"/>
-      <c r="CX11" s="47"/>
-      <c r="CY11" s="47"/>
-      <c r="CZ11" s="47"/>
-      <c r="DA11" s="47"/>
+      <c r="BY11" s="55"/>
+      <c r="BZ11" s="55"/>
+      <c r="CA11" s="55"/>
+      <c r="CB11" s="55"/>
+      <c r="CC11" s="55"/>
+      <c r="CD11" s="56"/>
+      <c r="CE11" s="44"/>
+      <c r="CF11" s="44"/>
+      <c r="CG11" s="44"/>
+      <c r="CH11" s="44"/>
+      <c r="CI11" s="44"/>
+      <c r="CJ11" s="44"/>
+      <c r="CK11" s="44"/>
+      <c r="CL11" s="44"/>
+      <c r="CM11" s="44"/>
+      <c r="CN11" s="44"/>
+      <c r="CO11" s="44"/>
+      <c r="CP11" s="44"/>
+      <c r="CQ11" s="44"/>
+      <c r="CR11" s="57"/>
+      <c r="CS11" s="57"/>
+      <c r="CT11" s="57"/>
+      <c r="CU11" s="44"/>
+      <c r="CV11" s="44"/>
+      <c r="CW11" s="44"/>
+      <c r="CX11" s="44"/>
+      <c r="CY11" s="44"/>
+      <c r="CZ11" s="44"/>
+      <c r="DA11" s="44"/>
     </row>
     <row r="12" spans="3:151" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M12" s="15"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="23"/>
-      <c r="AD12" s="23"/>
-      <c r="AE12" s="23"/>
-      <c r="AF12" s="23"/>
-      <c r="AG12" s="23"/>
-      <c r="AH12" s="23"/>
-      <c r="AI12" s="23"/>
-      <c r="AJ12" s="24"/>
-      <c r="AK12" s="40" t="s">
+      <c r="N12" s="38"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
+      <c r="V12" s="39"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39"/>
+      <c r="Z12" s="39"/>
+      <c r="AA12" s="39"/>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="39"/>
+      <c r="AD12" s="39"/>
+      <c r="AE12" s="39"/>
+      <c r="AF12" s="39"/>
+      <c r="AG12" s="39"/>
+      <c r="AH12" s="39"/>
+      <c r="AI12" s="39"/>
+      <c r="AJ12" s="40"/>
+      <c r="AK12" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="AL12" s="41"/>
-      <c r="AM12" s="41"/>
-      <c r="AN12" s="41"/>
-      <c r="AO12" s="41"/>
-      <c r="AP12" s="41"/>
-      <c r="AQ12" s="41"/>
-      <c r="AR12" s="41"/>
-      <c r="AS12" s="41"/>
-      <c r="AT12" s="41"/>
-      <c r="AU12" s="41"/>
-      <c r="AV12" s="41"/>
-      <c r="AW12" s="41"/>
-      <c r="AX12" s="41"/>
-      <c r="AY12" s="41"/>
-      <c r="AZ12" s="41"/>
-      <c r="BA12" s="41"/>
-      <c r="BB12" s="41"/>
-      <c r="BC12" s="41"/>
-      <c r="BD12" s="41"/>
-      <c r="BE12" s="41"/>
-      <c r="BF12" s="41"/>
-      <c r="BG12" s="41"/>
-      <c r="BH12" s="44" t="s">
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="23"/>
+      <c r="AN12" s="23"/>
+      <c r="AO12" s="23"/>
+      <c r="AP12" s="23"/>
+      <c r="AQ12" s="23"/>
+      <c r="AR12" s="23"/>
+      <c r="AS12" s="23"/>
+      <c r="AT12" s="23"/>
+      <c r="AU12" s="23"/>
+      <c r="AV12" s="23"/>
+      <c r="AW12" s="23"/>
+      <c r="AX12" s="23"/>
+      <c r="AY12" s="23"/>
+      <c r="AZ12" s="23"/>
+      <c r="BA12" s="23"/>
+      <c r="BB12" s="23"/>
+      <c r="BC12" s="23"/>
+      <c r="BD12" s="23"/>
+      <c r="BE12" s="23"/>
+      <c r="BF12" s="23"/>
+      <c r="BG12" s="23"/>
+      <c r="BH12" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="BI12" s="45"/>
-      <c r="BJ12" s="45"/>
-      <c r="BK12" s="45"/>
-      <c r="BL12" s="45"/>
-      <c r="BM12" s="45"/>
-      <c r="BN12" s="45"/>
-      <c r="BO12" s="45"/>
-      <c r="BP12" s="45"/>
-      <c r="BQ12" s="45"/>
-      <c r="BR12" s="45"/>
-      <c r="BS12" s="45"/>
-      <c r="BT12" s="45"/>
-      <c r="BU12" s="45"/>
-      <c r="BV12" s="45"/>
-      <c r="BW12" s="45"/>
-      <c r="BX12" s="45"/>
-      <c r="BY12" s="45"/>
-      <c r="BZ12" s="45"/>
-      <c r="CA12" s="45"/>
-      <c r="CB12" s="45"/>
-      <c r="CC12" s="45"/>
-      <c r="CD12" s="46"/>
-      <c r="CE12" s="47"/>
-      <c r="CF12" s="47"/>
-      <c r="CG12" s="47"/>
-      <c r="CH12" s="47"/>
-      <c r="CI12" s="47"/>
-      <c r="CJ12" s="47"/>
-      <c r="CK12" s="47"/>
-      <c r="CL12" s="47"/>
-      <c r="CM12" s="47"/>
-      <c r="CN12" s="47"/>
-      <c r="CO12" s="47"/>
-      <c r="CP12" s="47"/>
-      <c r="CQ12" s="47"/>
-      <c r="CR12" s="47"/>
-      <c r="CS12" s="47"/>
-      <c r="CT12" s="47"/>
-      <c r="CU12" s="47"/>
-      <c r="CV12" s="47"/>
-      <c r="CW12" s="47"/>
-      <c r="CX12" s="47"/>
-      <c r="CY12" s="47"/>
-      <c r="CZ12" s="47"/>
-      <c r="DA12" s="47"/>
+      <c r="BI12" s="42"/>
+      <c r="BJ12" s="42"/>
+      <c r="BK12" s="42"/>
+      <c r="BL12" s="42"/>
+      <c r="BM12" s="42"/>
+      <c r="BN12" s="42"/>
+      <c r="BO12" s="42"/>
+      <c r="BP12" s="42"/>
+      <c r="BQ12" s="42"/>
+      <c r="BR12" s="42"/>
+      <c r="BS12" s="42"/>
+      <c r="BT12" s="42"/>
+      <c r="BU12" s="42"/>
+      <c r="BV12" s="42"/>
+      <c r="BW12" s="42"/>
+      <c r="BX12" s="42"/>
+      <c r="BY12" s="42"/>
+      <c r="BZ12" s="42"/>
+      <c r="CA12" s="42"/>
+      <c r="CB12" s="42"/>
+      <c r="CC12" s="42"/>
+      <c r="CD12" s="43"/>
+      <c r="CE12" s="44"/>
+      <c r="CF12" s="44"/>
+      <c r="CG12" s="44"/>
+      <c r="CH12" s="44"/>
+      <c r="CI12" s="44"/>
+      <c r="CJ12" s="44"/>
+      <c r="CK12" s="44"/>
+      <c r="CL12" s="44"/>
+      <c r="CM12" s="44"/>
+      <c r="CN12" s="44"/>
+      <c r="CO12" s="44"/>
+      <c r="CP12" s="44"/>
+      <c r="CQ12" s="44"/>
+      <c r="CR12" s="44"/>
+      <c r="CS12" s="44"/>
+      <c r="CT12" s="44"/>
+      <c r="CU12" s="44"/>
+      <c r="CV12" s="44"/>
+      <c r="CW12" s="44"/>
+      <c r="CX12" s="44"/>
+      <c r="CY12" s="44"/>
+      <c r="CZ12" s="44"/>
+      <c r="DA12" s="44"/>
     </row>
     <row r="13" spans="3:151" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F13" s="14"/>
@@ -8085,6 +8086,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="N11:T11"/>
+    <mergeCell ref="U11:Z11"/>
+    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="AD11:AJ11"/>
     <mergeCell ref="N12:AJ12"/>
     <mergeCell ref="AK12:BG12"/>
     <mergeCell ref="BH12:CD12"/>
@@ -8101,11 +8107,6 @@
     <mergeCell ref="CL11:CQ11"/>
     <mergeCell ref="CR11:CT11"/>
     <mergeCell ref="CU11:DA11"/>
-    <mergeCell ref="C2:L2"/>
-    <mergeCell ref="N11:T11"/>
-    <mergeCell ref="U11:Z11"/>
-    <mergeCell ref="AA11:AC11"/>
-    <mergeCell ref="AD11:AJ11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>